<commit_message>
bold and new line in label
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/.xlsx
+++ b/xlsx/country_comparison/.xlsx
@@ -17,10 +17,10 @@
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">European Union</t>
+    <t xml:space="preserve">$ bold('All')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$ bold('European Union')</t>
   </si>
   <si>
     <t xml:space="preserve">United Kingdom</t>
@@ -48,20 +48,20 @@
     <t xml:space="preserve">Belief about GCS support in own country</t>
   </si>
   <si>
-    <t xml:space="preserve">Supports the GCS if its other members* cover 64-72% of world emissions
-*High: Global South + China + EU + various HICs (UK, Japan, South Korea, Canada...)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports the GCS if its other members* cover 64-72% of world emissions,
-*High color: High + Distributive effects displayed using colors on world map</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports the GCS if its other members* cover 56% of world emissions
-*Mid: Global South + China)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports the GCS if its other members* cover 25-33% of world emissions
-*Low: Global South + EU)</t>
+    <t xml:space="preserve">$ atop('                    Supports the GCS if its other members* cover 64-72% of world emissions', 
+                               '*' * bold(High) * ': Global South + China + EU + various HICs (UK, Japan, South Korea, Canada...)')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$ atop('     Supports the GCS if its other members* cover 64-72% of world emissions',          
+                                     '*' * bold('High color') * ': High + Distributive effects displayed using colors on world map')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$ atop('Supports the GCS if its other members* cover 56% of world emissions', 
+                              '                                                                   *' * bold('Mid') * ': Global South + China')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$ atop('Supports the GCS if its other members* cover 25-33% of world emissions', 
+                              '                                                                            *' * bold('Low') * ': Global South + EU')</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fix prepare field, render field
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/.xlsx
+++ b/xlsx/country_comparison/.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -53,23 +53,85 @@
     <t xml:space="preserve">USA</t>
   </si>
   <si>
-    <t xml:space="preserve">Supports tax on world top 1% to finance global poverty reduction
-(Additional 15% tax on income over [$120k/year in PPP])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports tax on world top 3% to finance global poverty reduction
-(Additional 15% tax over [$80k], 30% over [$120k], 45% over [$1M])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Governments should actively cooperate to have
-all countries converge in terms of GDP per capita by the end of the century"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports reparations for colonization and slavery in
-the form of funding education and technology transfers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"My taxes should go towards solving global problems"</t>
+    <t xml:space="preserve">Money; own income; cost of living; inflation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Relationships; love; emotions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Work; (un)employment; business</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poverty; inequality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global poverty; hunger; global inequality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Health; healthcare system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criticism of immigration; national preference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corruption; criticism of the government</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environment; climate change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Security; violence; crime; judicial system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discrimination; gender inequality; racism; LGBT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rights; democracy; freedom; slavery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happiness; peace of mind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">War; peace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tax system; welfare benefits; public services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criticism of far right; Trump; tariffs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social division; fake news; (social) media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animal welfare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Religion; sin; God</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Housing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Old age; retirement; ageing society</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family; children; childcare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International issues</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Own country referred</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other topic; unclear; vague</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nothing; don't know; empty</t>
   </si>
 </sst>
 </file>
@@ -447,40 +509,40 @@
         <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>0.25435325275351</v>
+        <v>0.176948673858409</v>
       </c>
       <c r="C2" t="n">
-        <v>0.229733730195768</v>
+        <v>0.155206454498852</v>
       </c>
       <c r="D2" t="n">
-        <v>0.247924142470634</v>
+        <v>0.165760187529138</v>
       </c>
       <c r="E2" t="n">
-        <v>0.238142009469067</v>
+        <v>0.132688996855489</v>
       </c>
       <c r="F2" t="n">
-        <v>0.143059479651997</v>
+        <v>0.170569645844742</v>
       </c>
       <c r="G2" t="n">
-        <v>0.217759808476751</v>
+        <v>0.179335609610556</v>
       </c>
       <c r="H2" t="n">
-        <v>0.228800388151237</v>
+        <v>0.13071460385036</v>
       </c>
       <c r="I2" t="n">
-        <v>0.271569064568047</v>
+        <v>0.167744724240085</v>
       </c>
       <c r="J2" t="n">
-        <v>0.348020929777486</v>
+        <v>0.121355113394281</v>
       </c>
       <c r="K2" t="n">
-        <v>0.195415895464876</v>
+        <v>0.148495010217095</v>
       </c>
       <c r="L2" t="n">
-        <v>0.151475972013406</v>
+        <v>0.217623806326528</v>
       </c>
       <c r="M2" t="n">
-        <v>0.308390049665346</v>
+        <v>0.231973932858366</v>
       </c>
     </row>
     <row r="3">
@@ -488,40 +550,40 @@
         <v>14</v>
       </c>
       <c r="B3" t="n">
-        <v>0.29487749862458</v>
+        <v>0.023746245554371</v>
       </c>
       <c r="C3" t="n">
-        <v>0.281518536195659</v>
+        <v>0.019454285576107</v>
       </c>
       <c r="D3" t="n">
-        <v>0.253607080882867</v>
+        <v>0.023277143708419</v>
       </c>
       <c r="E3" t="n">
-        <v>0.320972713411269</v>
+        <v>0.0207336999054023</v>
       </c>
       <c r="F3" t="n">
-        <v>0.249981556506401</v>
+        <v>0.0175328661238039</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2356708529277</v>
+        <v>0.0187877053768524</v>
       </c>
       <c r="H3" t="n">
-        <v>0.294159408870184</v>
+        <v>0.0178566210555686</v>
       </c>
       <c r="I3" t="n">
-        <v>0.272340441194078</v>
+        <v>0.0173152017198904</v>
       </c>
       <c r="J3" t="n">
-        <v>0.497083662868131</v>
+        <v>0.0194274400460883</v>
       </c>
       <c r="K3" t="n">
-        <v>0.286636713460478</v>
+        <v>0.00536727269964157</v>
       </c>
       <c r="L3" t="n">
-        <v>0.150456874440543</v>
+        <v>0.0460861309434834</v>
       </c>
       <c r="M3" t="n">
-        <v>0.331806163279924</v>
+        <v>0.0366365520055472</v>
       </c>
     </row>
     <row r="4">
@@ -529,40 +591,40 @@
         <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>0.260446615334856</v>
+        <v>0.038653527602944</v>
       </c>
       <c r="C4" t="n">
-        <v>0.187897042714528</v>
+        <v>0.0396355976118138</v>
       </c>
       <c r="D4" t="n">
-        <v>0.190489827374271</v>
+        <v>0.0488453402092147</v>
       </c>
       <c r="E4" t="n">
-        <v>0.205650306022925</v>
+        <v>0.0299275495122006</v>
       </c>
       <c r="F4" t="n">
-        <v>0.112376946594845</v>
+        <v>0.063182973582403</v>
       </c>
       <c r="G4" t="n">
-        <v>0.142081356516132</v>
+        <v>0.0293863348233816</v>
       </c>
       <c r="H4" t="n">
-        <v>0.135688096653865</v>
+        <v>0.048261771227565</v>
       </c>
       <c r="I4" t="n">
-        <v>0.287580264300726</v>
+        <v>0.0239296293435979</v>
       </c>
       <c r="J4" t="n">
-        <v>0.291140890930959</v>
+        <v>0.0158092268062042</v>
       </c>
       <c r="K4" t="n">
-        <v>0.240413858618638</v>
+        <v>0.0131676068923577</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0567640373741542</v>
+        <v>0.131664923797143</v>
       </c>
       <c r="M4" t="n">
-        <v>0.370153042354525</v>
+        <v>0.030113635988895</v>
       </c>
     </row>
     <row r="5">
@@ -570,32 +632,40 @@
         <v>16</v>
       </c>
       <c r="B5" t="n">
-        <v>0.422171960688106</v>
+        <v>0.072433196337855</v>
       </c>
       <c r="C5" t="n">
-        <v>0.385573018604744</v>
+        <v>0.0897430512402594</v>
       </c>
       <c r="D5" t="n">
-        <v>0.425132188839284</v>
+        <v>0.0815300483553539</v>
       </c>
       <c r="E5" t="n">
-        <v>0.428969403537556</v>
+        <v>0.108999927307447</v>
       </c>
       <c r="F5" t="n">
-        <v>0.243243479170587</v>
-      </c>
-      <c r="G5"/>
+        <v>0.0859696735401653</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.097729749508078</v>
+      </c>
       <c r="H5" t="n">
-        <v>0.390552355519347</v>
+        <v>0.0737373460322634</v>
       </c>
       <c r="I5" t="n">
-        <v>0.416880526453407</v>
-      </c>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
+        <v>0.0800897030643499</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.118689407285363</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.0707751809688699</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.0411491335889016</v>
+      </c>
       <c r="M5" t="n">
-        <v>0.457532301162332</v>
+        <v>0.0390959751910479</v>
       </c>
     </row>
     <row r="6">
@@ -603,40 +673,942 @@
         <v>17</v>
       </c>
       <c r="B6" t="n">
-        <v>0.281764207324566</v>
+        <v>0.0134410842070921</v>
       </c>
       <c r="C6" t="n">
-        <v>0.280799377736503</v>
+        <v>0.0166129673627565</v>
       </c>
       <c r="D6" t="n">
-        <v>0.426295117933464</v>
+        <v>0.00990324370778222</v>
       </c>
       <c r="E6" t="n">
-        <v>0.270461415958884</v>
+        <v>0.0100257576458049</v>
       </c>
       <c r="F6" t="n">
-        <v>0.157494415225418</v>
+        <v>0.0310965348388076</v>
       </c>
       <c r="G6" t="n">
-        <v>0.249815362045575</v>
+        <v>0.0187937296808294</v>
       </c>
       <c r="H6" t="n">
-        <v>0.20798277366565</v>
+        <v>0.0227853914465942</v>
       </c>
       <c r="I6" t="n">
-        <v>0.334776926213514</v>
+        <v>0.0130893432948986</v>
       </c>
       <c r="J6" t="n">
-        <v>0.337111171711107</v>
+        <v>0.0131440337020383</v>
       </c>
       <c r="K6" t="n">
-        <v>0.227457431436811</v>
+        <v>0.00511429124769571</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0828743570297473</v>
+        <v>0.00992595285253889</v>
       </c>
       <c r="M6" t="n">
-        <v>0.32215909520563</v>
+        <v>0.0101423291658875</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.119249582821528</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.136879279973913</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.120324740670292</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.109488055833458</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.155975584689061</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.138918781982572</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.16014865621119</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.155415205525748</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.116143119897375</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.058352512190181</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.0516680166571416</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.11496867295714</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.0440703328458708</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.0556835908767662</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0396349712847709</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.0821377590537621</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0287056885989428</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.0354198209688927</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.0340088165155789</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0909184296970719</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.0532106449141004</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.0158215408500238</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.00632678822322605</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.0355544106849215</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.0232845404949315</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0277190418004305</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0209335563539556</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.0187494817203833</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0144099090952224</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.0169933817648993</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.0818728898352045</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.0266003234543923</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.0131806164171693</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.0146937576608452</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.00526088777606903</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.0197410863201918</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0413945679478235</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0527612876240678</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0378478605827785</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.0640960220201268</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0754831299559596</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0221724636293523</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.0489547657952483</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.0515957186258728</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.0629643291809819</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.00995748759022352</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.0401051644319554</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.0284913632790919</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.0610075318045988</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.0682625497106202</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.11476818594713</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.0393363139888575</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.0848555762131242</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.0227930323951762</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.0633951364910317</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.0778012495096747</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.0350708572062188</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.0177302736228577</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.0392402832550644</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.065220313719315</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.036318313733475</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.0303492751701462</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.0305627962732717</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.0264317915553203</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.034093123900644</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0126742700578683</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.0254991210870382</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0443011694538446</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.0398784872706214</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.0281040310229985</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.0240291073428676</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.0550443378159004</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.0316619023583936</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.020167126115703</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.012436959125538</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.015254879727607</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0240251118972616</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0136802596231349</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.0167572994369076</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.0341142180962793</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.0414125956620657</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.0278375740358052</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.037357798631603</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.0577809170495888</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.0270711259919894</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.0310465966023829</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.0254065753213864</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.0174198071731154</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.0473346575981105</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0164898986204219</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.017704736977718</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.057995023038915</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.0269991451826757</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.0128543543549344</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.0218472473238587</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.0245978902847182</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.0606381063267319</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.0847187754510992</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.0514829203403444</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.113468714902909</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.122399066294443</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.116752665308591</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.0547975117455974</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.0478921388154982</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.100305476507664</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.0149209786920427</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.0588883645207161</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.0243221311329973</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.0715444499861098</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.0742247482511581</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.0968802933753493</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.0653488341490191</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.0669329178080904</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.0373841093051816</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.0514033398038403</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.110932848292568</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.0509445319215343</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.160236623877362</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.00259584218681808</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.0427086483595602</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.0438713209812911</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.0229189727406162</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0203047890339714</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.0378843527230824</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0189346000174674</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.0130491389225625</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.00951853360227524</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.026871057567979</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.0141139196218575</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.0333209351965288</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.102941226332114</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.00912296727788547</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.0090905907641623</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.00861603556073884</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.0147080327277219</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.00654357988851507</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.00536247626473339</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.011106023696502</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.00464674298425364</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.0148563509789483</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.00114312378109044</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.00779960431154217</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.012504935511294</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.00548439090212051</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.00738544044333992</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.00842704851418689</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.0106175169548618</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.00535221128258067</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.0110870113292001</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.0031425168348546</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.00471247697531813</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.00984903169908945</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.00111540434016411</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0.00421941073126723</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.00903084455774402</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.00350747267813929</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.00240140039481314</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.00301388411452899</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.0026974301047993</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.0092221941939587</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.00406859162073066</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.00175842094182187</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.00375924498514015</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.0427657775628182</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.017558389011036</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.0299395379640607</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.0307080033339235</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0239433045098027</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.0159204887615089</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.0209681437129943</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.0281447893994951</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.0653390788490106</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.0421129108189791</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0.0253025873266461</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.00600177916881286</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.0344377143298887</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.0374342235485173</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.0225570852665277</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.0242247062909054</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.0127877887089121</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.038101941816959</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0173965795919296</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.0102241499270583</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.0388779572908386</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.0198134289823329</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.0378033562142717</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.0155109272498332</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.0514429547160629</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.0161626898189773</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.0323250644293763</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.0332771655305157</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.0288447172197366</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.0695657997417108</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0133416408178441</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.0134564935505487</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.026229722760271</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.0271151403596097</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.0280780210661461</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.071711581519768</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.0112898831610919</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.0179785869922492</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.0473249104815912</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.0480314017698516</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0513258945872917</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.0257853652953644</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.0585395107540181</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.046207997690817</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.0425554224405343</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.0707934688656888</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.0315922988317157</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.0521321802651446</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.0760092820323943</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.0390763141446832</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.0389666735972933</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.0460228362443624</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0528611468776913</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.048095279732958</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.051046397560614</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.0498480559610093</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.0380105738124306</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.0364497278863142</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.0392455795985156</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.0160678239474841</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.0541528634172794</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.029048691788262</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.0216536003001745</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.0248207347219647</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.0163511671350575</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.0485662219745389</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.0112276432244119</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.0358078413818051</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.0191124040881251</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.0157885681956608</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.00599281533977228</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.011539037887782</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.0128482567735397</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.0197595653702909</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.127140761791366</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.104596364579166</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.121129745948714</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.0784908462762879</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.105397921368922</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.120168576782413</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.102948798652095</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.109001218234964</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.132777811109319</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.182170110782153</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.180026939982192</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.145992376067682</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.0932294855086049</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.0918378018291469</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.0983621789594571</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.128972183901413</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.052217230565829</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.114297886560459</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0.0729564800276328</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0.0709886380284247</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0.122372587777753</v>
+      </c>
+      <c r="K28" t="n">
+        <v>0.150484018727778</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.0807607818857155</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.0763595325583267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
conjoint better size, nolabel
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/.xlsx
+++ b/xlsx/country_comparison/.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -53,15 +53,33 @@
     <t xml:space="preserve">USA</t>
   </si>
   <si>
+    <t xml:space="preserve">Supports tax on world top 1% to finance global poverty reduction
+(Additional 15% tax on income over [$120k/year in PPP])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports tax on world top 3% to finance global poverty reduction
+(Additional 15% tax over [$80k], 30% over [$120k], 45% over [$1M])</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prefers sustainable future</t>
   </si>
   <si>
-    <t xml:space="preserve">Prefers sustainable future
-(Variant: Scenario A = Sustainable)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prefers sustainable future
-(Variant: Scenario B = Sustainable)</t>
+    <t xml:space="preserve">"Governments should actively cooperate to have
+all countries converge in terms of GDP per capita by the end of the century"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Could sign a petition and spread ideas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More likely to vote for party if part of worldwide
+coalition for climate action and global redistribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports reparations for colonization and slavery in
+the form of funding education and technology transfers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"My taxes should go towards solving global problems"</t>
   </si>
 </sst>
 </file>
@@ -439,40 +457,40 @@
         <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>0.679366394096195</v>
+        <v>0.244781082578977</v>
       </c>
       <c r="C2" t="n">
-        <v>0.701539116816613</v>
+        <v>0.237490071485306</v>
       </c>
       <c r="D2" t="n">
-        <v>0.721220700610069</v>
+        <v>0.243781094527363</v>
       </c>
       <c r="E2" t="n">
-        <v>0.703415187125182</v>
+        <v>0.242201834862385</v>
       </c>
       <c r="F2" t="n">
-        <v>0.759706650286704</v>
+        <v>0.145118733509235</v>
       </c>
       <c r="G2" t="n">
-        <v>0.575101001313061</v>
+        <v>0.219512195121951</v>
       </c>
       <c r="H2" t="n">
-        <v>0.731116681894394</v>
+        <v>0.218354430379747</v>
       </c>
       <c r="I2" t="n">
-        <v>0.683377424047149</v>
+        <v>0.277777777777778</v>
       </c>
       <c r="J2" t="n">
-        <v>0.659704988708263</v>
+        <v>0.341880341880342</v>
       </c>
       <c r="K2" t="n">
-        <v>0.759423291434471</v>
+        <v>0.2</v>
       </c>
       <c r="L2" t="n">
-        <v>0.721853509181885</v>
+        <v>0.157446808510638</v>
       </c>
       <c r="M2" t="n">
-        <v>0.618615448895168</v>
+        <v>0.315463917525773</v>
       </c>
     </row>
     <row r="3">
@@ -480,40 +498,40 @@
         <v>14</v>
       </c>
       <c r="B3" t="n">
-        <v>0.693628531000139</v>
+        <v>0.288705924467514</v>
       </c>
       <c r="C3" t="n">
-        <v>0.720085595824866</v>
+        <v>0.295729250604351</v>
       </c>
       <c r="D3" t="n">
-        <v>0.736984879434596</v>
+        <v>0.252525252525253</v>
       </c>
       <c r="E3" t="n">
-        <v>0.725881595869102</v>
+        <v>0.312127236580517</v>
       </c>
       <c r="F3" t="n">
-        <v>0.765907100909998</v>
+        <v>0.254641909814324</v>
       </c>
       <c r="G3" t="n">
-        <v>0.611889231338192</v>
+        <v>0.240157480314961</v>
       </c>
       <c r="H3" t="n">
-        <v>0.743424508873319</v>
+        <v>0.289198606271777</v>
       </c>
       <c r="I3" t="n">
-        <v>0.704613116707588</v>
+        <v>0.267441860465116</v>
       </c>
       <c r="J3" t="n">
-        <v>0.658773642965459</v>
+        <v>0.519148936170213</v>
       </c>
       <c r="K3" t="n">
-        <v>0.757102957447094</v>
+        <v>0.284466019417476</v>
       </c>
       <c r="L3" t="n">
-        <v>0.815436145072691</v>
+        <v>0.145283018867925</v>
       </c>
       <c r="M3" t="n">
-        <v>0.623296468364111</v>
+        <v>0.329449838187702</v>
       </c>
     </row>
     <row r="4">
@@ -521,40 +539,235 @@
         <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>0.664640848496477</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.68320853906189</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.702621358461442</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.685046818395573</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.754990230010101</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.532316461825255</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.729425485286049</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.651605593520223</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.672192292694225</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.758873295962316</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>0.598082915941509</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.609951253611223</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.240272727272727</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1972</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.18546365914787</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.21087786259542</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.113756613756614</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.142</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.139303482587065</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.288135593220339</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.294243070362473</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.242</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.063</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.1704</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.171679197994987</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.157442748091603</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.111111111111111</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.166</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.129353233830846</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.174334140435835</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.232409381663113</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.1765</v>
+      </c>
+      <c r="L7"/>
+      <c r="M7" t="n">
+        <v>0.183666666666667</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.414450291565922</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.384271892830563</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.422305764411028</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.425572519083969</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.247354497354497</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" t="n">
+        <v>0.386401326699834</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.418886198547215</v>
+      </c>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8" t="n">
+        <v>0.455</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.266363636363636</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.2838</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.422305764411028</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.270038167938931</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.16005291005291</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.203980099502488</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.328087167070218</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.345415778251599</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.227</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.322333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
custom_redistr (determinants, fig), corr fields, labels
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/.xlsx
+++ b/xlsx/country_comparison/.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -20,85 +20,64 @@
     <t xml:space="preserve">$ bold('All')</t>
   </si>
   <si>
-    <t xml:space="preserve">Millionaires</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Europe Non-voters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Europe Left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Europe Center/Right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Europe Far right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japan Non-voters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japan Left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japan Center/Right</t>
+    <t xml:space="preserve">$ bold('Europe')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switzerland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japan</t>
   </si>
   <si>
     <t xml:space="preserve">Saudi Arabia</t>
   </si>
   <si>
-    <t xml:space="preserve">Saudi citizens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U.S. Non-voters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U.S. Harris</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U.S. Trump</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports the National Climate Scheme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Global climate scheme (GCS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports int'l climate scheme (any variant)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports int'l tax on millionaires
-with 30% funding LICs (any variant)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports tax on world top 1% to finance global poverty reduction
-(Additional 15% tax on income over [$120k/year in PPP])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports tax on world top 3% to finance global poverty reduction
-(Additional 15% tax over [$80k], 30% over [$120k], 45% over [$1M])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prefers sustainable future</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Governments should actively cooperate to have
-all countries converge in terms of GDP per capita by the end of the century"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Could sign a petition and spread ideas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">More likely to vote for party if part of worldwide
-coalition for climate action and global redistribution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports reparations for colonization and slavery in
-the form of funding education and technology transfers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"My taxes should go towards solving global problems"</t>
+    <t xml:space="preserve">USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferred share of winners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferred share of losers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preferred degree of redistribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implied minimum income (in $/year)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implied transfer (in % of world income)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am satisfied with my custom redistribution.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I want to skip this question.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has not touched the sliders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Touched sliders and satisfied</t>
   </si>
 </sst>
 </file>
@@ -470,561 +449,374 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>0.664226512802836</v>
+        <v>47.3738987802139</v>
       </c>
       <c r="C2" t="n">
-        <v>0.572848551968255</v>
+        <v>47.9271661362879</v>
       </c>
       <c r="D2" t="n">
-        <v>0.644575228658036</v>
+        <v>47.235101025608</v>
       </c>
       <c r="E2" t="n">
-        <v>0.800284739031995</v>
+        <v>46.5056769193759</v>
       </c>
       <c r="F2" t="n">
-        <v>0.642550167034555</v>
+        <v>48.7201520505185</v>
       </c>
       <c r="G2" t="n">
-        <v>0.469492339511511</v>
+        <v>49.4760424962276</v>
       </c>
       <c r="H2" t="n">
-        <v>0.686245500193959</v>
+        <v>49.0283360313302</v>
       </c>
       <c r="I2" t="n">
-        <v>0.693180009940773</v>
+        <v>48.4130854078035</v>
       </c>
       <c r="J2" t="n">
-        <v>0.70121194589928</v>
+        <v>44.7857599076557</v>
       </c>
       <c r="K2" t="n">
-        <v>0.880240645828153</v>
+        <v>46.7817073785458</v>
       </c>
       <c r="L2" t="n">
-        <v>0.909247309965247</v>
+        <v>49.8918139075144</v>
       </c>
       <c r="M2" t="n">
-        <v>0.635891200808388</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0.784787411820172</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0.496232098818529</v>
+        <v>46.7542391167642</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="n">
-        <v>0.564056918460414</v>
+        <v>17.7284309346652</v>
       </c>
       <c r="C3" t="n">
-        <v>0.438519909819211</v>
+        <v>17.6757157738403</v>
       </c>
       <c r="D3" t="n">
-        <v>0.608336262307662</v>
+        <v>18.4467406250294</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7742661541532</v>
+        <v>17.483715865681</v>
       </c>
       <c r="F3" t="n">
-        <v>0.599498572230777</v>
+        <v>17.2320852638926</v>
       </c>
       <c r="G3" t="n">
-        <v>0.458263840559057</v>
+        <v>16.754096665448</v>
       </c>
       <c r="H3" t="n">
-        <v>0.484301365259412</v>
+        <v>18.4623046745572</v>
       </c>
       <c r="I3" t="n">
-        <v>0.612085827792447</v>
+        <v>17.4189241105924</v>
       </c>
       <c r="J3" t="n">
-        <v>0.572309112554739</v>
+        <v>18.3851242687856</v>
       </c>
       <c r="K3" t="n">
-        <v>0.845249604687817</v>
+        <v>17.7384550005227</v>
       </c>
       <c r="L3" t="n">
-        <v>0.851579637309937</v>
+        <v>17.4538497656465</v>
       </c>
       <c r="M3" t="n">
-        <v>0.53634538292824</v>
-      </c>
-      <c r="N3" t="n">
-        <v>0.578812451569643</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.351976770537292</v>
+        <v>17.8088827749863</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="n">
-        <v>0.66651612376134</v>
+        <v>4.66215828721021</v>
       </c>
       <c r="C4" t="n">
-        <v>0.573361650550744</v>
+        <v>4.81863675290261</v>
       </c>
       <c r="D4" t="n">
-        <v>0.667007243291184</v>
+        <v>4.62639569404863</v>
       </c>
       <c r="E4" t="n">
-        <v>0.846305654167647</v>
+        <v>4.64029111788804</v>
       </c>
       <c r="F4" t="n">
-        <v>0.708488851215913</v>
+        <v>5.15669116783075</v>
       </c>
       <c r="G4" t="n">
-        <v>0.545881515572153</v>
+        <v>4.91824763267677</v>
       </c>
       <c r="H4" t="n">
-        <v>0.613467393904764</v>
+        <v>5.02493311213579</v>
       </c>
       <c r="I4" t="n">
-        <v>0.747738543210677</v>
+        <v>4.77084250692855</v>
       </c>
       <c r="J4" t="n">
-        <v>0.687280315653707</v>
+        <v>4.42395634859103</v>
       </c>
       <c r="K4" t="n">
-        <v>0.879515634668033</v>
+        <v>4.54104222019968</v>
       </c>
       <c r="L4" t="n">
-        <v>0.911224469217849</v>
+        <v>4.98006182286059</v>
       </c>
       <c r="M4" t="n">
-        <v>0.626914750584237</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.751213818870576</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.425296011477573</v>
+        <v>4.50342546995902</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5" t="n">
-        <v>0.698602594648788</v>
+        <v>2904.13174396868</v>
       </c>
       <c r="C5" t="n">
-        <v>0.406090627387198</v>
+        <v>3013.99648441846</v>
       </c>
       <c r="D5" t="n">
-        <v>0.723594997027424</v>
+        <v>2856.27218254474</v>
       </c>
       <c r="E5" t="n">
-        <v>0.889579981493868</v>
+        <v>2866.37646927345</v>
       </c>
       <c r="F5" t="n">
-        <v>0.682683457496027</v>
+        <v>3268.67955624125</v>
       </c>
       <c r="G5" t="n">
-        <v>0.589211476424677</v>
+        <v>3174.89746134272</v>
       </c>
       <c r="H5" t="n">
-        <v>0.601734056180248</v>
+        <v>3168.21066966258</v>
       </c>
       <c r="I5" t="n">
-        <v>0.736254582714072</v>
+        <v>2966.48272925279</v>
       </c>
       <c r="J5" t="n">
-        <v>0.678198041159092</v>
+        <v>2660.91125126678</v>
       </c>
       <c r="K5" t="n">
-        <v>0.832453270416735</v>
+        <v>2791.36080801827</v>
       </c>
       <c r="L5" t="n">
-        <v>0.831456137791045</v>
+        <v>3291.56572730894</v>
       </c>
       <c r="M5" t="n">
-        <v>0.685388571356183</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.792944541873363</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0.496524297223254</v>
+        <v>2789.12603881073</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="n">
-        <v>0.548749204972874</v>
+        <v>5.11274339194611</v>
       </c>
       <c r="C6" t="n">
-        <v>0.366613390750273</v>
+        <v>5.39514273808263</v>
       </c>
       <c r="D6" t="n">
-        <v>0.583987178202389</v>
+        <v>5.0147638962913</v>
       </c>
       <c r="E6" t="n">
-        <v>0.809444964341555</v>
+        <v>5.10885958685904</v>
       </c>
       <c r="F6" t="n">
-        <v>0.502893565174609</v>
+        <v>5.93329114050014</v>
       </c>
       <c r="G6" t="n">
-        <v>0.484386429576709</v>
+        <v>5.86127261939289</v>
       </c>
       <c r="H6" t="n">
-        <v>0.356013330649719</v>
+        <v>5.65083244023413</v>
       </c>
       <c r="I6" t="n">
-        <v>0.508382107274219</v>
+        <v>5.28587527204688</v>
       </c>
       <c r="J6" t="n">
-        <v>0.451398568187944</v>
+        <v>4.66029346746541</v>
       </c>
       <c r="K6" t="n">
-        <v>0.677827112481047</v>
+        <v>4.6584932524887</v>
       </c>
       <c r="L6" t="n">
-        <v>0.743498584988873</v>
+        <v>5.91408224230056</v>
       </c>
       <c r="M6" t="n">
-        <v>0.503559387678212</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.636870250532107</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.373907558453907</v>
+        <v>4.89938812724382</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="n">
-        <v>0.488009346515533</v>
+        <v>0.557747404615879</v>
       </c>
       <c r="C7" t="n">
-        <v>0.304486035670833</v>
+        <v>0.581924165984681</v>
       </c>
       <c r="D7" t="n">
-        <v>0.513014491525721</v>
+        <v>0.528351073871356</v>
       </c>
       <c r="E7" t="n">
-        <v>0.71931115965366</v>
+        <v>0.568251340340844</v>
       </c>
       <c r="F7" t="n">
-        <v>0.495264748486105</v>
+        <v>0.633294813075585</v>
       </c>
       <c r="G7" t="n">
-        <v>0.440316456384772</v>
+        <v>0.56683869430922</v>
       </c>
       <c r="H7" t="n">
-        <v>0.342128267431882</v>
+        <v>0.627561397537583</v>
       </c>
       <c r="I7" t="n">
-        <v>0.454830804343478</v>
+        <v>0.586565171659253</v>
       </c>
       <c r="J7" t="n">
-        <v>0.306878691636744</v>
+        <v>0.541107445542664</v>
       </c>
       <c r="K7" t="n">
-        <v>0.671355992475847</v>
+        <v>0.396397500500417</v>
       </c>
       <c r="L7" t="n">
-        <v>0.73716679715381</v>
+        <v>0.675626482239489</v>
       </c>
       <c r="M7" t="n">
-        <v>0.45566201329143</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.566039039099673</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.339022055208755</v>
+        <v>0.583598508969987</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" t="n">
-        <v>0.679366394096195</v>
+        <v>0.429455777564688</v>
       </c>
       <c r="C8" t="n">
-        <v>0.595648253088616</v>
+        <v>0.399938028884069</v>
       </c>
       <c r="D8" t="n">
-        <v>0.680987204503282</v>
+        <v>0.444355939422213</v>
       </c>
       <c r="E8" t="n">
-        <v>0.831184500933943</v>
+        <v>0.413791210382809</v>
       </c>
       <c r="F8" t="n">
-        <v>0.695788344040076</v>
+        <v>0.347683813345704</v>
       </c>
       <c r="G8" t="n">
-        <v>0.538162773640089</v>
+        <v>0.423972329239059</v>
       </c>
       <c r="H8" t="n">
-        <v>0.743500976587183</v>
+        <v>0.354534285584268</v>
       </c>
       <c r="I8" t="n">
-        <v>0.81462228490617</v>
+        <v>0.400478141047647</v>
       </c>
       <c r="J8" t="n">
-        <v>0.756962294490717</v>
+        <v>0.434832711547606</v>
       </c>
       <c r="K8" t="n">
-        <v>0.713280127381035</v>
+        <v>0.592104616524749</v>
       </c>
       <c r="L8" t="n">
-        <v>0.703520370125625</v>
+        <v>0.324134427552624</v>
       </c>
       <c r="M8" t="n">
-        <v>0.671406780430398</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.776812968723143</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.425499404919733</v>
+        <v>0.408076772619088</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" t="n">
-        <v>0.582407081968796</v>
+        <v>0.408374634826883</v>
       </c>
       <c r="C9" t="n">
-        <v>0.440671030859726</v>
+        <v>0.388588909468523</v>
       </c>
       <c r="D9" t="n">
-        <v>0.616661919613841</v>
+        <v>0.399590058385227</v>
       </c>
       <c r="E9" t="n">
-        <v>0.791367358009102</v>
+        <v>0.384091647511391</v>
       </c>
       <c r="F9" t="n">
-        <v>0.647850068391449</v>
+        <v>0.410195834228784</v>
       </c>
       <c r="G9" t="n">
-        <v>0.562087374904841</v>
+        <v>0.302872499149178</v>
       </c>
       <c r="H9" t="n">
-        <v>0.529885434677782</v>
+        <v>0.371813108427663</v>
       </c>
       <c r="I9" t="n">
-        <v>0.619694338952137</v>
+        <v>0.437136028711529</v>
       </c>
       <c r="J9" t="n">
-        <v>0.581289088318094</v>
+        <v>0.303667681206425</v>
       </c>
       <c r="K9" t="n">
-        <v>0.756844881931732</v>
+        <v>0.475448989690047</v>
       </c>
       <c r="L9" t="n">
-        <v>0.822839088961434</v>
+        <v>0.388366284732463</v>
       </c>
       <c r="M9" t="n">
-        <v>0.529363660067618</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.581144289159245</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.389096341662054</v>
+        <v>0.406177169426307</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" t="n">
-        <v>0.517681293588919</v>
+        <v>0.398118456901027</v>
       </c>
       <c r="C10" t="n">
-        <v>0.37450861498383</v>
+        <v>0.410488474534835</v>
       </c>
       <c r="D10" t="n">
-        <v>0.54400229948967</v>
+        <v>0.369081820440341</v>
       </c>
       <c r="E10" t="n">
-        <v>0.661278534958537</v>
+        <v>0.430038380653647</v>
       </c>
       <c r="F10" t="n">
-        <v>0.497096533902024</v>
+        <v>0.410781068299679</v>
       </c>
       <c r="G10" t="n">
-        <v>0.442405137881287</v>
+        <v>0.459008243270367</v>
       </c>
       <c r="H10" t="n">
-        <v>0.389456592496737</v>
+        <v>0.427013225872613</v>
       </c>
       <c r="I10" t="n">
-        <v>0.639772161098881</v>
+        <v>0.380331129442371</v>
       </c>
       <c r="J10" t="n">
-        <v>0.541929639804469</v>
+        <v>0.455290253425317</v>
       </c>
       <c r="K10" t="n">
-        <v>0.404576421408372</v>
+        <v>0.279967106328976</v>
       </c>
       <c r="L10" t="n">
-        <v>0.407592835762763</v>
+        <v>0.442866209980246</v>
       </c>
       <c r="M10" t="n">
-        <v>0.489892191381658</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0.654584229780058</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0.324832521986835</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.364700740506257</v>
-      </c>
-      <c r="C11" t="n">
-        <v>0.301437840047023</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0.347757564445013</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.612564469882184</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0.329076922032927</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0.266032348749018</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.163374634470308</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.313128420422624</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.218439546291854</v>
-      </c>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11" t="n">
-        <v>0.282837312902432</v>
-      </c>
-      <c r="N11" t="n">
-        <v>0.521302744077032</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0.271064836019934</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="n">
-        <v>0.347856888878235</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.261828422049271</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.393011358029993</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0.540846531529226</v>
-      </c>
-      <c r="F12" t="n">
-        <v>0.30076097129752</v>
-      </c>
-      <c r="G12" t="n">
-        <v>0.236110214107178</v>
-      </c>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12" t="n">
-        <v>0.31201873214884</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.450138037793688</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0.174002494177101</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="n">
-        <v>0.414163491723958</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.396411998512916</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.37990538035527</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.606618681027554</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0.404741669455715</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0.296470179474792</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.282576495496765</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0.376409725924188</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.325947806714271</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0.662536527281334</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0.698489352155402</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.362460536490887</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.536101382797469</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0.265773612275098</v>
+        <v>0.426810711448192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug ru council
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/.xlsx
+++ b/xlsx/country_comparison/.xlsx
@@ -56,23 +56,24 @@
     <t xml:space="preserve">USA</t>
   </si>
   <si>
-    <t xml:space="preserve">Supports tax on world top 1% to finance global poverty reduction
-(Additional 15% tax on income over [$120k/year in PPP])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports tax on world top 3% to finance global poverty reduction
-(Additional 15% tax over [$80k], 30% over [$120k], 45% over [$1M])</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Governments should actively cooperate to have all countries
-converge in terms of GDP per capita by the end of the century"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports reparations for colonization and slavery in
-the form of funding education and technology transfers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"My taxes should go towards solving global problems"</t>
+    <t xml:space="preserve">Bridgetown initiative: MDBs expanding sustainable
+investments in LICs, and at lower interest rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L&amp;D: Developed countries financing a fund to help
+vulnerable countries cope with climate Loss and damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NCQG: Developing countries providing $300 bn a
+year in climate finance for developing countries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International levy on shipping carbon emissions,
+returned to countries based on population</t>
+  </si>
+  <si>
+    <t xml:space="preserve">International levy on aviation carbon emissions, raising
+prices by 30%, returned to countries based on population</t>
   </si>
 </sst>
 </file>
@@ -453,43 +454,43 @@
         <v>14</v>
       </c>
       <c r="B2" t="n">
-        <v>0.245639138393658</v>
+        <v>0.146010599841289</v>
       </c>
       <c r="C2" t="n">
-        <v>0.229733730195768</v>
+        <v>0.132542332167995</v>
       </c>
       <c r="D2" t="n">
-        <v>0.247924142470634</v>
+        <v>0.129596752130756</v>
       </c>
       <c r="E2" t="n">
-        <v>0.238142009469067</v>
+        <v>0.145675582853815</v>
       </c>
       <c r="F2" t="n">
-        <v>0.143059479651997</v>
+        <v>0.0954243293657346</v>
       </c>
       <c r="G2" t="n">
-        <v>0.217759808476751</v>
+        <v>0.187103716184443</v>
       </c>
       <c r="H2" t="n">
-        <v>0.228800388151237</v>
+        <v>0.133718785954441</v>
       </c>
       <c r="I2" t="n">
-        <v>0.271569064568047</v>
+        <v>0.11492056193604</v>
       </c>
       <c r="J2" t="n">
-        <v>0.348020929777486</v>
+        <v>0.200694966921401</v>
       </c>
       <c r="K2" t="n">
-        <v>0.195415895464876</v>
+        <v>0.108934797301173</v>
       </c>
       <c r="L2" t="n">
-        <v>0.195290010165635</v>
+        <v>0.115957534266233</v>
       </c>
       <c r="M2" t="n">
-        <v>0.151475972013406</v>
+        <v>0.103803725511012</v>
       </c>
       <c r="N2" t="n">
-        <v>0.308390049665346</v>
+        <v>0.190645354507088</v>
       </c>
     </row>
     <row r="3">
@@ -497,43 +498,43 @@
         <v>15</v>
       </c>
       <c r="B3" t="n">
-        <v>0.280225312927298</v>
+        <v>0.183841010690089</v>
       </c>
       <c r="C3" t="n">
-        <v>0.281518536195659</v>
+        <v>0.194778464468711</v>
       </c>
       <c r="D3" t="n">
-        <v>0.253607080882867</v>
+        <v>0.213864747902659</v>
       </c>
       <c r="E3" t="n">
-        <v>0.320972713411269</v>
+        <v>0.201130669827433</v>
       </c>
       <c r="F3" t="n">
-        <v>0.249981556506401</v>
+        <v>0.133480638057468</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2356708529277</v>
+        <v>0.215369575310077</v>
       </c>
       <c r="H3" t="n">
-        <v>0.294159408870184</v>
+        <v>0.182926447567268</v>
       </c>
       <c r="I3" t="n">
-        <v>0.272340441194078</v>
+        <v>0.211859250596182</v>
       </c>
       <c r="J3" t="n">
-        <v>0.497083662868131</v>
+        <v>0.259238044125371</v>
       </c>
       <c r="K3" t="n">
-        <v>0.286636713460478</v>
+        <v>0.165272179682437</v>
       </c>
       <c r="L3" t="n">
-        <v>0.182880051386794</v>
+        <v>0.0871473725545981</v>
       </c>
       <c r="M3" t="n">
-        <v>0.150456874440543</v>
+        <v>0.0889994868827042</v>
       </c>
       <c r="N3" t="n">
-        <v>0.331806163279924</v>
+        <v>0.223983980933038</v>
       </c>
     </row>
     <row r="4">
@@ -541,43 +542,43 @@
         <v>16</v>
       </c>
       <c r="B4" t="n">
-        <v>0.254374248643458</v>
+        <v>0.224855569886564</v>
       </c>
       <c r="C4" t="n">
-        <v>0.187897042714528</v>
+        <v>0.237091536063245</v>
       </c>
       <c r="D4" t="n">
-        <v>0.190489827374271</v>
+        <v>0.242630093096098</v>
       </c>
       <c r="E4" t="n">
-        <v>0.205650306022925</v>
+        <v>0.242386252480975</v>
       </c>
       <c r="F4" t="n">
-        <v>0.112376946594845</v>
+        <v>0.198545795017619</v>
       </c>
       <c r="G4" t="n">
-        <v>0.142081356516132</v>
+        <v>0.269549366392053</v>
       </c>
       <c r="H4" t="n">
-        <v>0.135688096653865</v>
+        <v>0.197009596906079</v>
       </c>
       <c r="I4" t="n">
-        <v>0.287580264300726</v>
+        <v>0.256785775713629</v>
       </c>
       <c r="J4" t="n">
-        <v>0.291140890930959</v>
+        <v>0.293560168251507</v>
       </c>
       <c r="K4" t="n">
-        <v>0.240413858618638</v>
+        <v>0.224573726058832</v>
       </c>
       <c r="L4" t="n">
-        <v>0.216312281488782</v>
+        <v>0.0875701282476831</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0567640373741542</v>
+        <v>0.110540387994507</v>
       </c>
       <c r="N4" t="n">
-        <v>0.370153042354525</v>
+        <v>0.273750099644573</v>
       </c>
     </row>
     <row r="5">
@@ -585,33 +586,43 @@
         <v>17</v>
       </c>
       <c r="B5" t="n">
-        <v>0.422171960688106</v>
+        <v>0.202578438222928</v>
       </c>
       <c r="C5" t="n">
-        <v>0.385573018604744</v>
+        <v>0.196948123102502</v>
       </c>
       <c r="D5" t="n">
-        <v>0.425132188839284</v>
+        <v>0.169168517949569</v>
       </c>
       <c r="E5" t="n">
-        <v>0.428969403537556</v>
+        <v>0.212277412820648</v>
       </c>
       <c r="F5" t="n">
-        <v>0.243243479170587</v>
-      </c>
-      <c r="G5"/>
+        <v>0.174659754267382</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.283705683005757</v>
+      </c>
       <c r="H5" t="n">
-        <v>0.390552355519347</v>
+        <v>0.192021566228126</v>
       </c>
       <c r="I5" t="n">
-        <v>0.416880526453407</v>
-      </c>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
+        <v>0.179181000868458</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.219418118627448</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.211370747417242</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.17153412063256</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.137132444050968</v>
+      </c>
       <c r="N5" t="n">
-        <v>0.457532301162332</v>
+        <v>0.222593638315052</v>
       </c>
     </row>
     <row r="6">
@@ -619,43 +630,43 @@
         <v>18</v>
       </c>
       <c r="B6" t="n">
-        <v>0.282824123860505</v>
+        <v>0.335896829807718</v>
       </c>
       <c r="C6" t="n">
-        <v>0.280799377736503</v>
+        <v>0.348129936326248</v>
       </c>
       <c r="D6" t="n">
-        <v>0.426295117933464</v>
+        <v>0.291303617905378</v>
       </c>
       <c r="E6" t="n">
-        <v>0.270461415958884</v>
+        <v>0.351914348414487</v>
       </c>
       <c r="F6" t="n">
-        <v>0.157494415225418</v>
+        <v>0.360761234851986</v>
       </c>
       <c r="G6" t="n">
-        <v>0.249815362045575</v>
+        <v>0.350961918380286</v>
       </c>
       <c r="H6" t="n">
-        <v>0.20798277366565</v>
+        <v>0.36078150758704</v>
       </c>
       <c r="I6" t="n">
-        <v>0.334776926213514</v>
+        <v>0.357671887298782</v>
       </c>
       <c r="J6" t="n">
-        <v>0.337111171711107</v>
+        <v>0.405003093387077</v>
       </c>
       <c r="K6" t="n">
-        <v>0.227457431436811</v>
+        <v>0.305275672060071</v>
       </c>
       <c r="L6" t="n">
-        <v>0.28868736465168</v>
+        <v>0.323298223558926</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0828743570297473</v>
+        <v>0.233843638288844</v>
       </c>
       <c r="N6" t="n">
-        <v>0.32215909520563</v>
+        <v>0.347584039700156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
top_tax_affected, world income tax revenue
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/.xlsx
+++ b/xlsx/country_comparison/.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t xml:space="preserve">Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia</t>
   </si>
   <si>
     <t xml:space="preserve">Saudi Arabia</t>
@@ -57,7 +60,7 @@
 (Any variant)</t>
   </si>
   <si>
-    <t xml:space="preserve">Affected by the (variant faced of the) top tax</t>
+    <t xml:space="preserve">Affected by the top tax (any variant)</t>
   </si>
   <si>
     <t xml:space="preserve">Supports tax on world top 1% to finance global poverty reduction
@@ -443,51 +446,57 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="n">
-        <v>0.458655202633503</v>
+        <v>0.562249333952068</v>
       </c>
       <c r="C2" t="n">
         <v>0.530633111073681</v>
       </c>
       <c r="D2" t="n">
-        <v>0.728060762438549</v>
+        <v>0.534615441391404</v>
       </c>
       <c r="E2" t="n">
-        <v>0.433277453890483</v>
+        <v>0.532199124020193</v>
       </c>
       <c r="F2" t="n">
-        <v>0.670220829481084</v>
+        <v>0.475339526743875</v>
       </c>
       <c r="G2" t="n">
-        <v>0.500997266398559</v>
+        <v>0.455066177183276</v>
       </c>
       <c r="H2" t="n">
-        <v>0.354532209125533</v>
+        <v>0.481053473314213</v>
       </c>
       <c r="I2" t="n">
-        <v>0.554162668358118</v>
+        <v>0.644527456241547</v>
       </c>
       <c r="J2" t="n">
-        <v>0.381407423879945</v>
+        <v>0.283838350853901</v>
       </c>
       <c r="K2" t="n">
-        <v>0.312651458927067</v>
+        <v>0.278766736483527</v>
       </c>
       <c r="L2" t="n">
-        <v>0.637081457535834</v>
+        <v>0.599907829518252</v>
       </c>
       <c r="M2" t="n">
-        <v>0.44754651248597</v>
+        <v>0.695880953418338</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.38602041410698</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" t="n">
         <v>0.0591524213077198</v>
@@ -519,57 +528,61 @@
       <c r="K3" t="n">
         <v>0.0300920300421565</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3"/>
+      <c r="M3" t="n">
         <v>0.213457131326528</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>0.0779223306659385</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="n">
-        <v>0.528888358626659</v>
+        <v>0.593568464643459</v>
       </c>
       <c r="C4" t="n">
         <v>0.623206921829844</v>
       </c>
       <c r="D4" t="n">
-        <v>0.759306272998927</v>
+        <v>0.662100661962385</v>
       </c>
       <c r="E4" t="n">
-        <v>0.455234037906956</v>
+        <v>0.645129138499509</v>
       </c>
       <c r="F4" t="n">
-        <v>0.646319884351791</v>
+        <v>0.652088141940814</v>
       </c>
       <c r="G4" t="n">
         <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>0.638361679043372</v>
+        <v>0.595169320047074</v>
       </c>
       <c r="I4" t="n">
-        <v>0.492036390872307</v>
+        <v>0.581049693515047</v>
       </c>
       <c r="J4" t="n">
-        <v>0.650144217307684</v>
+        <v>0.460003610927742</v>
       </c>
       <c r="K4" t="n">
-        <v>0.418169519433632</v>
+        <v>0.321840723174092</v>
       </c>
       <c r="L4" t="n">
-        <v>0.522951617509147</v>
+        <v>0.599907829518252</v>
       </c>
       <c r="M4" t="n">
-        <v>0.489850782983131</v>
+        <v>0.656234738255263</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.466960372968151</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="n">
         <v>0.0324192263079185</v>
@@ -578,80 +591,84 @@
         <v>0.0228809019118487</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0168076927398806</v>
+        <v>0.0152772811251959</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0156399541396257</v>
+        <v>0.0158159265407275</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0379209062301266</v>
+        <v>0.0364460596482764</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00539414658045392</v>
+        <v>0.00635212756481645</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0135134355442693</v>
+        <v>0.013703147356521</v>
       </c>
       <c r="I5" t="n">
-        <v>0.0387987232432794</v>
+        <v>0.0382299828227781</v>
       </c>
       <c r="J5" t="n">
-        <v>0.06987857565294</v>
+        <v>0.0699523880243387</v>
       </c>
       <c r="K5" t="n">
-        <v>0.0191985328268543</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.132205913258965</v>
-      </c>
+        <v>0.0195161254114759</v>
+      </c>
+      <c r="L5"/>
       <c r="M5" t="n">
-        <v>0.0409323300541326</v>
+        <v>0.136800251123575</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.0397521568871045</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B6" t="n">
-        <v>0.432729011460262</v>
+        <v>0.564833073218838</v>
       </c>
       <c r="C6" t="n">
         <v>0.494229631325223</v>
       </c>
       <c r="D6" t="n">
-        <v>0.694652395845772</v>
+        <v>0.494509481529061</v>
       </c>
       <c r="E6" t="n">
-        <v>0.622665668771534</v>
+        <v>0.482293276239211</v>
       </c>
       <c r="F6" t="n">
-        <v>0.548482144697428</v>
+        <v>0.377478972984925</v>
       </c>
       <c r="G6" t="n">
-        <v>0.434789042286224</v>
+        <v>0.317062120727541</v>
       </c>
       <c r="H6" t="n">
-        <v>0.376672900705601</v>
+        <v>0.446739876773781</v>
       </c>
       <c r="I6" t="n">
-        <v>0.610651971508659</v>
+        <v>0.666981999539339</v>
       </c>
       <c r="J6" t="n">
-        <v>0.231936795277737</v>
+        <v>0.204001758620865</v>
       </c>
       <c r="K6" t="n">
-        <v>0.333000333000333</v>
+        <v>0.259051167955435</v>
       </c>
       <c r="L6" t="n">
-        <v>0.676810040857224</v>
+        <v>0.599907829518252</v>
       </c>
       <c r="M6" t="n">
-        <v>0.369319480210762</v>
+        <v>0.713245760172143</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.359482567475819</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="n">
         <v>0.085037992635904</v>
@@ -660,34 +677,35 @@
         <v>0.058871310106645</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0460874543518805</v>
+        <v>0.0497557537097689</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0411657855802637</v>
+        <v>0.0381284684121215</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0660744172057993</v>
+        <v>0.0651357948522902</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0231861533967205</v>
+        <v>0.0243920108908461</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0483308966472912</v>
+        <v>0.0494954076529742</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0953377939181177</v>
+        <v>0.0998345665218679</v>
       </c>
       <c r="J7" t="n">
-        <v>0.165895078203565</v>
+        <v>0.160672303258471</v>
       </c>
       <c r="K7" t="n">
-        <v>0.042539129854292</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.294709996866589</v>
-      </c>
+        <v>0.0400180177711981</v>
+      </c>
+      <c r="L7"/>
       <c r="M7" t="n">
-        <v>0.113010172525853</v>
+        <v>0.282886812048479</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.113725803486659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
re-run RU 1001; without crop
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/.xlsx
+++ b/xlsx/country_comparison/.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -59,22 +59,47 @@
     <t xml:space="preserve">U.S. Trump</t>
   </si>
   <si>
-    <t xml:space="preserve">Latent support
-for global redistribution (standardized)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share of plausible global policies supported</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share of plausible global policies opposed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Difference between share of plausible
-policies supported and opposed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ratio of share of plausible policies
-supported over supported or opposed</t>
+    <t xml:space="preserve">Supports the National Climate Scheme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Global climate scheme (GCS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports int'l climate scheme (any variant)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports int'l tax on millionaires
+with 30% funding LICs (any variant)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports tax on world top 1% to finance global poverty reduction
+(Additional 15% tax on income over [$120k/year in PPP])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports tax on world top 3% to finance global poverty reduction
+(Additional 15% tax over [$80k], 30% over [$120k], 45% over [$1M])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prefers sustainable future</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Governments should actively cooperate to have all countries
+converge in terms of GDP per capita by the end of the century"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would support a global movement to tackle CC, tax millionaires,
+ and fund LICs (either petition, demonstrate, strike, or donate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More likely to vote for party if part of worldwide
+coalition for climate action and global redistribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports reparations for colonization and slavery in
+the form of funding education and technology transfers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"My taxes should go towards solving global problems"</t>
   </si>
 </sst>
 </file>
@@ -458,46 +483,46 @@
         <v>15</v>
       </c>
       <c r="B2" t="n">
-        <v>0.118072592422114</v>
+        <v>0.678255122017956</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.0498367465468193</v>
+        <v>0.582213755593942</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0900466965070292</v>
+        <v>0.644575228658036</v>
       </c>
       <c r="E2" t="n">
-        <v>0.773249073043927</v>
+        <v>0.800284739031995</v>
       </c>
       <c r="F2" t="n">
-        <v>0.169433490463815</v>
+        <v>0.642550167034555</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.398894953418106</v>
+        <v>0.469492339511511</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.323601595472413</v>
+        <v>0.686368170390751</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0450127982223677</v>
+        <v>0.693214710621706</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.129567448417396</v>
+        <v>0.701245337266761</v>
       </c>
       <c r="K2" t="n">
-        <v>0.570613442792331</v>
+        <v>0.880240645828153</v>
       </c>
       <c r="L2" t="n">
-        <v>0.703893156336886</v>
+        <v>0.909247309965247</v>
       </c>
       <c r="M2" t="n">
-        <v>-0.108149019641461</v>
+        <v>0.636149633119223</v>
       </c>
       <c r="N2" t="n">
-        <v>0.538844686201452</v>
+        <v>0.785390250556912</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.544785197190979</v>
+        <v>0.496956252308101</v>
       </c>
     </row>
     <row r="3">
@@ -505,46 +530,46 @@
         <v>16</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5</v>
+        <v>0.553746767090015</v>
       </c>
       <c r="C3" t="n">
-        <v>0.5</v>
+        <v>0.452808231861887</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5</v>
+        <v>0.608336262307662</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8</v>
+        <v>0.7742661541532</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6</v>
+        <v>0.599498572230777</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4</v>
+        <v>0.458263840559057</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2</v>
+        <v>0.484321597862702</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>0.612111541228833</v>
       </c>
       <c r="J3" t="n">
-        <v>0.4</v>
+        <v>0.572331454255148</v>
       </c>
       <c r="K3" t="n">
-        <v>0.7</v>
+        <v>0.846428606188793</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8</v>
+        <v>0.851579637309937</v>
       </c>
       <c r="M3" t="n">
-        <v>0.4</v>
+        <v>0.536291385483281</v>
       </c>
       <c r="N3" t="n">
-        <v>0.7</v>
+        <v>0.579183059294616</v>
       </c>
       <c r="O3" t="n">
-        <v>0.3</v>
+        <v>0.352117596369122</v>
       </c>
     </row>
     <row r="4">
@@ -552,46 +577,46 @@
         <v>17</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1</v>
+        <v>0.655683473250087</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2</v>
+        <v>0.579787314673126</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1</v>
+        <v>0.667007243291184</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.846305654167647</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1</v>
+        <v>0.708488851215913</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3</v>
+        <v>0.545881515572153</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1</v>
+        <v>0.613538232894647</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1</v>
+        <v>0.74780131987402</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1</v>
+        <v>0.687363838387126</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>0.87796797988428</v>
       </c>
       <c r="L4" t="n">
-        <v>0</v>
+        <v>0.911224469217849</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1</v>
+        <v>0.627010199560514</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>0.75157471671655</v>
       </c>
       <c r="O4" t="n">
-        <v>0.3</v>
+        <v>0.425288098957725</v>
       </c>
     </row>
     <row r="5">
@@ -599,46 +624,46 @@
         <v>18</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4</v>
+        <v>0.704079856692946</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3</v>
+        <v>0.426801076374466</v>
       </c>
       <c r="D5" t="n">
-        <v>0.3</v>
+        <v>0.723594997027424</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7</v>
+        <v>0.889579981493869</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4</v>
+        <v>0.682683457496027</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1</v>
+        <v>0.589211476424677</v>
       </c>
       <c r="H5" t="n">
-        <v>0.1</v>
+        <v>0.601842995962143</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3</v>
+        <v>0.736252789377503</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2</v>
+        <v>0.678172368299312</v>
       </c>
       <c r="K5" t="n">
-        <v>0.6</v>
+        <v>0.830395038048113</v>
       </c>
       <c r="L5" t="n">
-        <v>0.7</v>
+        <v>0.831456137791045</v>
       </c>
       <c r="M5" t="n">
-        <v>0.2</v>
+        <v>0.685485640466168</v>
       </c>
       <c r="N5" t="n">
-        <v>0.6</v>
+        <v>0.793249457133825</v>
       </c>
       <c r="O5" t="n">
-        <v>0</v>
+        <v>0.496836260204527</v>
       </c>
     </row>
     <row r="6">
@@ -646,46 +671,361 @@
         <v>19</v>
       </c>
       <c r="B6" t="n">
-        <v>0.857142857142857</v>
+        <v>0.556565037682828</v>
       </c>
       <c r="C6" t="n">
-        <v>0.777777777777778</v>
+        <v>0.393016824439431</v>
       </c>
       <c r="D6" t="n">
-        <v>0.833333333333333</v>
+        <v>0.583987178202389</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0.809444964341555</v>
       </c>
       <c r="F6" t="n">
-        <v>0.857142857142857</v>
+        <v>0.502893565174609</v>
       </c>
       <c r="G6" t="n">
-        <v>0.6</v>
+        <v>0.484386429576709</v>
       </c>
       <c r="H6" t="n">
-        <v>0.75</v>
+        <v>0.356105750421195</v>
       </c>
       <c r="I6" t="n">
-        <v>0.857142857142857</v>
+        <v>0.508432438341536</v>
       </c>
       <c r="J6" t="n">
-        <v>0.777777777777778</v>
+        <v>0.451519556659133</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9</v>
+        <v>0.677827112481047</v>
       </c>
       <c r="L6" t="n">
-        <v>1</v>
+        <v>0.743498584988873</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8</v>
+        <v>0.503741905167505</v>
       </c>
       <c r="N6" t="n">
-        <v>1</v>
+        <v>0.637096655800029</v>
       </c>
       <c r="O6" t="n">
-        <v>0.5</v>
+        <v>0.373993319775201</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.503247309719211</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.316231358914818</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.513014491525721</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.71931115965366</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.495264748486105</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.440316456384772</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.34215953895184</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.455068700122256</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.306824263084082</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.671355992475847</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.73716679715381</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.455679906453223</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.566496834134014</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.339067925103543</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.680815013747804</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.616668833076667</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.680987204503282</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.831184500933943</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.695788344040076</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.538162773640089</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.743644347389163</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.814701212857562</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.757048871605567</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.721853509181885</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.703520370125625</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.671270631778761</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.776836935461012</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.425661149175785</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.704960018034767</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.501381130731594</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.787483813023996</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.876770446811719</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.74609538238357</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.664878143534609</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.7335602187152</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.725922165695082</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.685126203737904</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.92816201896394</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.938466265662205</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.688883535477258</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.68963486840272</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.436451458600216</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.675595447215337</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.523930159271177</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.709363981944143</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.892471876813608</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.637051467662211</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.578161277543308</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.433349195600366</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.696851480613757</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.583790255087382</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.729122438104651</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.741985444624183</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.641824096726743</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.834461320073758</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.474126518973143</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.364717906507653</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.301242387158432</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.347757564445013</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.612564469882184</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.329076922032927</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.266032348749018</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.163327499246366</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.313179598308858</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.218483573122562</v>
+      </c>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11" t="n">
+        <v>0.283095421815601</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.52122515690493</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.27084855688435</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.347853243460036</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.262527011404327</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.393011358029993</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.540846531529226</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.30076097129752</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.236110214107178</v>
+      </c>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12" t="n">
+        <v>0.311745273790548</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.450524011973634</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.173904958357855</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.410629863862209</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.393225264575894</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.37990538035527</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.606618681027554</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.404741669455715</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.296470179474792</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.282669471326983</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.376571407830385</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.32600471502799</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.665815836537034</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.698489352155402</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.362475436951784</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.535384805366787</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.265617828927838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove fast RU, crop, plot HTML in plot_along using laptop ggplot2 3.5.1
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/.xlsx
+++ b/xlsx/country_comparison/.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -23,55 +23,67 @@
     <t xml:space="preserve">$ bold('Europe')</t>
   </si>
   <si>
+    <t xml:space="preserve">France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switzerland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia</t>
+  </si>
+  <si>
     <t xml:space="preserve">Saudi Arabia</t>
   </si>
   <si>
-    <t xml:space="preserve">Italy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Germany</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Kingdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Russia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poland</t>
-  </si>
-  <si>
     <t xml:space="preserve">USA</t>
   </si>
   <si>
-    <t xml:space="preserve">Switzerland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latent support
-for global redistribution (standardized)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share of plausible global policies supported</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share of plausible global policies opposed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Difference between share of plausible
-policies supported and opposed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ratio of share of plausible policies
-supported over supported or opposed</t>
+    <t xml:space="preserve">Supports tax on world top 1% to finance global poverty reduction
+(Additional 15% tax on income over [$120k/year in PPP])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports tax on world top 3% to finance global poverty reduction
+(Additional 15% tax over [$80k], 30% over [$120k], 45% over [$1M])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prefers sustainable future</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Governments should actively cooperate to have all countries
+converge in terms of GDP per capita by the end of the century"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would support a global movement to tackle CC, tax millionaires,
+ and fund LICs (either petition, demonstrate, strike, or donate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More likely to vote for party if part of worldwide
+coalition for climate action and global redistribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supports reparations for colonization and slavery in
+the form of funding education and technology transfers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"My taxes should go towards solving global problems"</t>
   </si>
 </sst>
 </file>
@@ -452,43 +464,43 @@
         <v>14</v>
       </c>
       <c r="B2" t="n">
-        <v>0.118266759376858</v>
+        <v>0.241205184312405</v>
       </c>
       <c r="C2" t="n">
-        <v>0.27483374700023</v>
+        <v>0.237490071485306</v>
       </c>
       <c r="D2" t="n">
-        <v>0.570091796525703</v>
+        <v>0.243781094527363</v>
       </c>
       <c r="E2" t="n">
-        <v>0.555677179146155</v>
+        <v>0.242201834862385</v>
       </c>
       <c r="F2" t="n">
-        <v>0.429169099523955</v>
+        <v>0.145118733509235</v>
       </c>
       <c r="G2" t="n">
-        <v>0.222911418354213</v>
+        <v>0.219512195121951</v>
       </c>
       <c r="H2" t="n">
-        <v>0.232606439940633</v>
+        <v>0.218354430379747</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0625930589717066</v>
+        <v>0.277777777777778</v>
       </c>
       <c r="J2" t="n">
-        <v>0.176715138826425</v>
+        <v>0.341880341880342</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0288229401824224</v>
+        <v>0.2</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0910009593694564</v>
+        <v>0.204545454545455</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0246363044895293</v>
+        <v>0.157446808510638</v>
       </c>
       <c r="N2" t="n">
-        <v>-0.180817852873774</v>
+        <v>0.315463917525773</v>
       </c>
     </row>
     <row r="3">
@@ -496,43 +508,43 @@
         <v>15</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5</v>
+        <v>0.281590234246123</v>
       </c>
       <c r="C3" t="n">
-        <v>0.6</v>
+        <v>0.295729250604351</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7</v>
+        <v>0.252525252525253</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7</v>
+        <v>0.312127236580517</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7</v>
+        <v>0.254641909814324</v>
       </c>
       <c r="G3" t="n">
-        <v>0.6</v>
+        <v>0.240157480314961</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6</v>
+        <v>0.289198606271777</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5</v>
+        <v>0.267441860465116</v>
       </c>
       <c r="J3" t="n">
-        <v>0.6</v>
+        <v>0.519148936170213</v>
       </c>
       <c r="K3" t="n">
-        <v>0.5</v>
+        <v>0.284466019417476</v>
       </c>
       <c r="L3" t="n">
-        <v>0.5</v>
+        <v>0.197894736842105</v>
       </c>
       <c r="M3" t="n">
-        <v>0.5</v>
+        <v>0.145283018867925</v>
       </c>
       <c r="N3" t="n">
-        <v>0.4</v>
+        <v>0.329449838187702</v>
       </c>
     </row>
     <row r="4">
@@ -540,43 +552,43 @@
         <v>16</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.111111111111111</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -584,43 +596,43 @@
         <v>17</v>
       </c>
       <c r="B5" t="n">
-        <v>0.4</v>
+        <v>0.279180423383181</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5</v>
+        <v>0.22951582867784</v>
       </c>
       <c r="D5" t="n">
-        <v>0.6</v>
+        <v>0.231611893583725</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6</v>
+        <v>0.246376811594203</v>
       </c>
       <c r="F5" t="n">
-        <v>0.5</v>
+        <v>0.12778603268945</v>
       </c>
       <c r="G5" t="n">
-        <v>0.5</v>
+        <v>0.156043956043956</v>
       </c>
       <c r="H5" t="n">
-        <v>0.5</v>
+        <v>0.158790170132325</v>
       </c>
       <c r="I5" t="n">
-        <v>0.333333333333333</v>
+        <v>0.340974212034384</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4</v>
+        <v>0.340740740740741</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3</v>
+        <v>0.298397040690506</v>
       </c>
       <c r="L5" t="n">
-        <v>0.3</v>
+        <v>0.231768231768232</v>
       </c>
       <c r="M5" t="n">
-        <v>0.3</v>
+        <v>0.0743801652892562</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2</v>
+        <v>0.438388625592417</v>
       </c>
     </row>
     <row r="6">
@@ -628,43 +640,159 @@
         <v>18</v>
       </c>
       <c r="B6" t="n">
-        <v>0.857142857142857</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>0.875</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.888888888888889</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0.857142857142857</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0.875</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.833333333333333</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.833333333333333</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L6"/>
       <c r="M6" t="n">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>0.777777777777778</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.1704</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.171679197994987</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.157442748091603</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.111111111111111</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.166</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.129353233830846</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.174334140435835</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.232409381663113</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.1765</v>
+      </c>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7" t="n">
+        <v>0.183666666666667</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.414450291565922</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.384271892830563</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.422305764411028</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.425572519083969</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.247354497354497</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" t="n">
+        <v>0.386401326699834</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.418886198547215</v>
+      </c>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8" t="n">
+        <v>0.455</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.268977585201233</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.2838</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.422305764411028</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.270038167938931</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.16005291005291</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.244</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.203980099502488</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.328087167070218</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.345415778251599</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.227</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.297702297702298</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.322333333333333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support -> accept in figs
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/.xlsx
+++ b/xlsx/country_comparison/.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -56,24 +56,34 @@
     <t xml:space="preserve">USA</t>
   </si>
   <si>
-    <t xml:space="preserve">Supports tax on world top 1% to finance global poverty reduction
+    <t xml:space="preserve">Accepts tax on world top 1% to finance global poverty reduction
 (Additional 15% tax on income over [$120k/year in PPP])</t>
   </si>
   <si>
-    <t xml:space="preserve">Percentage of fellow citizens affected by top 1% tax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of GDP transferred abroad in top 1% tax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supports tax on world top 3% to finance global poverty reduction
+    <t xml:space="preserve">Accepts tax on world top 3% to finance global poverty reduction
 (Additional 15% tax over [$80k], 30% over [$120k], 45% over [$1M])</t>
   </si>
   <si>
-    <t xml:space="preserve">Percentage of fellow citizens affected by top 3% tax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of GDP transferred abroad in top 3% tax</t>
+    <t xml:space="preserve">Prefers sustainable future</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Governments should actively cooperate to have all countries
+converge in terms of GDP per capita by the end of the century"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would support a global movement to tackle CC, tax millionaires,
+ and fund LICs (either petition, demonstrate, strike, or donate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More likely to vote for party if part of worldwide
+coalition for climate action and global redistribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accepts reparations for colonization and slavery in
+the form of funding education and technology transfers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"My taxes should go towards solving global problems"</t>
   </si>
 </sst>
 </file>
@@ -454,43 +464,43 @@
         <v>14</v>
       </c>
       <c r="B2" t="n">
-        <v>0.245412103741306</v>
+        <v>0.692894784662911</v>
       </c>
       <c r="C2" t="n">
-        <v>0.229733730195768</v>
+        <v>0.709953011533533</v>
       </c>
       <c r="D2" t="n">
-        <v>0.247924142470634</v>
+        <v>0.694020071682012</v>
       </c>
       <c r="E2" t="n">
-        <v>0.238142009469067</v>
+        <v>0.716874917652575</v>
       </c>
       <c r="F2" t="n">
-        <v>0.143059479651997</v>
+        <v>0.817931401759025</v>
       </c>
       <c r="G2" t="n">
-        <v>0.217759808476751</v>
+        <v>0.688331328542526</v>
       </c>
       <c r="H2" t="n">
-        <v>0.228800388151237</v>
+        <v>0.727696489623426</v>
       </c>
       <c r="I2" t="n">
-        <v>0.271569064568047</v>
+        <v>0.680287179370093</v>
       </c>
       <c r="J2" t="n">
-        <v>0.348020929777486</v>
+        <v>0.611054424765204</v>
       </c>
       <c r="K2" t="n">
-        <v>0.195364903919637</v>
+        <v>0.667587247975338</v>
       </c>
       <c r="L2" t="n">
-        <v>0.195245846345785</v>
+        <v>0.734266953673365</v>
       </c>
       <c r="M2" t="n">
-        <v>0.151475972013406</v>
+        <v>0.816793423425975</v>
       </c>
       <c r="N2" t="n">
-        <v>0.308420535787809</v>
+        <v>0.613078913946868</v>
       </c>
     </row>
     <row r="3">
@@ -498,43 +508,43 @@
         <v>15</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0480768816457684</v>
+        <v>0.648431801604668</v>
       </c>
       <c r="C3" t="n">
-        <v>0.02852787093506</v>
+        <v>0.654418197725284</v>
       </c>
       <c r="D3" t="n">
-        <v>0.02</v>
+        <v>0.69867423579194</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04</v>
+        <v>0.631062611744521</v>
       </c>
       <c r="F3" t="n">
-        <v>0.02</v>
+        <v>0.71347266445345</v>
       </c>
       <c r="G3" t="n">
-        <v>0.02</v>
+        <v>0.698563809102872</v>
       </c>
       <c r="H3" t="n">
-        <v>0.02</v>
+        <v>0.668248725994209</v>
       </c>
       <c r="I3" t="n">
-        <v>0.04</v>
+        <v>0.688695322348303</v>
       </c>
       <c r="J3" t="n">
-        <v>0.04</v>
+        <v>0.412823621757237</v>
       </c>
       <c r="K3" t="n">
-        <v>0.04</v>
+        <v>0.548789112211414</v>
       </c>
       <c r="L3" t="n">
-        <v>0.02</v>
+        <v>0.745575769472929</v>
       </c>
       <c r="M3" t="n">
-        <v>0.11</v>
+        <v>0.820236659115239</v>
       </c>
       <c r="N3" t="n">
-        <v>0.08</v>
+        <v>0.587193769163202</v>
       </c>
     </row>
     <row r="4">
@@ -542,43 +552,43 @@
         <v>16</v>
       </c>
       <c r="B4" t="n">
-        <v>0.01996694788084</v>
+        <v>0.664778686805119</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0122599357880939</v>
+        <v>0.680960854092527</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01</v>
+        <v>0.701612903225806</v>
       </c>
       <c r="E4" t="n">
-        <v>0.02</v>
+        <v>0.683610867659947</v>
       </c>
       <c r="F4" t="n">
-        <v>0.01</v>
+        <v>0.728285077951002</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01</v>
+        <v>0.568822553897181</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01</v>
+        <v>0.726299694189602</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01</v>
+        <v>0.667752442996743</v>
       </c>
       <c r="J4" t="n">
-        <v>0.01</v>
+        <v>0.65607476635514</v>
       </c>
       <c r="K4" t="n">
-        <v>0.01</v>
+        <v>0.706269349845201</v>
       </c>
       <c r="L4" t="n">
-        <v>0.02</v>
+        <v>0.685934489402698</v>
       </c>
       <c r="M4" t="n">
-        <v>0.05</v>
+        <v>0.668763102725367</v>
       </c>
       <c r="N4" t="n">
-        <v>0.03</v>
+        <v>0.602535832414553</v>
       </c>
     </row>
     <row r="5">
@@ -586,43 +596,43 @@
         <v>17</v>
       </c>
       <c r="B5" t="n">
-        <v>0.281236083230862</v>
+        <v>0.705793226381462</v>
       </c>
       <c r="C5" t="n">
-        <v>0.281518536195659</v>
+        <v>0.7602300376023</v>
       </c>
       <c r="D5" t="n">
-        <v>0.253607080882867</v>
+        <v>0.762917933130699</v>
       </c>
       <c r="E5" t="n">
-        <v>0.320972713411269</v>
+        <v>0.740149094781683</v>
       </c>
       <c r="F5" t="n">
-        <v>0.249981556506401</v>
+        <v>0.856145251396648</v>
       </c>
       <c r="G5" t="n">
-        <v>0.2356708529277</v>
+        <v>0.825301204819277</v>
       </c>
       <c r="H5" t="n">
-        <v>0.294159408870184</v>
+        <v>0.830601092896175</v>
       </c>
       <c r="I5" t="n">
-        <v>0.272340441194078</v>
+        <v>0.652413793103448</v>
       </c>
       <c r="J5" t="n">
-        <v>0.497083662868131</v>
+        <v>0.658256880733945</v>
       </c>
       <c r="K5" t="n">
-        <v>0.286766411013822</v>
+        <v>0.663065843621399</v>
       </c>
       <c r="L5" t="n">
-        <v>0.192189650223197</v>
+        <v>0.765895953757225</v>
       </c>
       <c r="M5" t="n">
-        <v>0.150456874440543</v>
+        <v>0.917480998914224</v>
       </c>
       <c r="N5" t="n">
-        <v>0.331670856933351</v>
+        <v>0.555436337625179</v>
       </c>
     </row>
     <row r="6">
@@ -630,43 +640,43 @@
         <v>18</v>
       </c>
       <c r="B6" t="n">
-        <v>0.105924471185012</v>
+        <v>0.611777124330845</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0633468330019907</v>
+        <v>0.672953736654804</v>
       </c>
       <c r="D6" t="n">
-        <v>0.05</v>
+        <v>0.668202764976959</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1</v>
+        <v>0.670464504820333</v>
       </c>
       <c r="F6" t="n">
-        <v>0.05</v>
+        <v>0.736080178173719</v>
       </c>
       <c r="G6" t="n">
-        <v>0.04</v>
+        <v>0.648424543946932</v>
       </c>
       <c r="H6" t="n">
-        <v>0.05</v>
+        <v>0.723241590214067</v>
       </c>
       <c r="I6" t="n">
-        <v>0.05</v>
+        <v>0.642779587404995</v>
       </c>
       <c r="J6" t="n">
-        <v>0.18</v>
+        <v>0.598130841121495</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1</v>
+        <v>0.506191950464396</v>
       </c>
       <c r="L6" t="n">
-        <v>0.04</v>
+        <v>0.506191950464396</v>
       </c>
       <c r="M6" t="n">
-        <v>0.16</v>
+        <v>0.560447239692523</v>
       </c>
       <c r="N6" t="n">
-        <v>0.18</v>
+        <v>0.612458654906284</v>
       </c>
     </row>
     <row r="7">
@@ -674,43 +684,117 @@
         <v>19</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0536797711265189</v>
+        <v>0.664188137644821</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0315155900509169</v>
+        <v>0.711714770797963</v>
       </c>
       <c r="D7" t="n">
-        <v>0.02</v>
+        <v>0.710578842315369</v>
       </c>
       <c r="E7" t="n">
-        <v>0.04</v>
+        <v>0.705192629815745</v>
       </c>
       <c r="F7" t="n">
-        <v>0.03</v>
+        <v>0.801272507913065</v>
       </c>
       <c r="G7" t="n">
-        <v>0.04</v>
+        <v>0.646090534979424</v>
       </c>
       <c r="H7" t="n">
-        <v>0.03</v>
+        <v>0.769662921348315</v>
       </c>
       <c r="I7" t="n">
-        <v>0.03</v>
+        <v>0.693877551020408</v>
       </c>
       <c r="J7" t="n">
-        <v>0.03</v>
+        <v>0.58695652173913</v>
       </c>
       <c r="K7" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.12</v>
-      </c>
+        <v>0.515331355093966</v>
+      </c>
+      <c r="L7"/>
+      <c r="M7"/>
       <c r="N7" t="n">
-        <v>0.08</v>
+        <v>0.669950738916256</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.461188014718766</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.502795031055901</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.436893203883495</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.442563482466747</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.685958024097665</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8" t="n">
+        <v>0.511201629327902</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.461068702290076</v>
+      </c>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8" t="n">
+        <v>0.407318053880177</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.622476446837147</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.612353567625133</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.441176470588235</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.62962962962963</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.771253333873262</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.641833810888252</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.712018140589569</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.584084084084084</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.532786885245902</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.601431980906921</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.577994428969359</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.882267286664075</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.571005917159763</v>
       </c>
     </row>
   </sheetData>

</xml_diff>